<commit_message>
added scripts directory to 2017-etnp
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-mclane-profile.xlsx
+++ b/analyses/etnp2017-p2-mclane-profile.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35B4B3A-367C-9147-9E34-F0894549E8DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA3EA50-5499-9E41-86C2-8CB4AA1C1245}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="640" windowWidth="28040" windowHeight="14680" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="300" yWindow="560" windowWidth="25600" windowHeight="14640" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="MED4" sheetId="17" r:id="rId2"/>
+    <sheet name="all data" sheetId="1" r:id="rId1"/>
+    <sheet name="100-965 comparison" sheetId="17" r:id="rId2"/>
     <sheet name="ptm" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="99">
   <si>
     <t>Sample running #</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>ID'd proteins</t>
-  </si>
-  <si>
-    <t>de novo only spectra</t>
   </si>
   <si>
     <t>NT1:2-9_94m_topnw1</t>
@@ -290,9 +287,6 @@
     <t>% DNO peptides modified</t>
   </si>
   <si>
-    <t>Cyano DNO sequences</t>
-  </si>
-  <si>
     <t>Depth (m)</t>
   </si>
   <si>
@@ -325,12 +319,39 @@
       <t xml:space="preserve"> pool</t>
     </r>
   </si>
+  <si>
+    <t>de novo only spectra &gt; 50%</t>
+  </si>
+  <si>
+    <t>Suspended 2.7&gt;GF75&gt;0.3</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinking </t>
+  </si>
+  <si>
+    <t>NT1:2-9_94m_topnw1+4</t>
+  </si>
+  <si>
+    <t>NT5:4-19_965m_nw1+4</t>
+  </si>
+  <si>
+    <t>de novo only peptides &gt; 50% ALC</t>
+  </si>
+  <si>
+    <t>de novo only peptides &gt; 50% ALC (ave)</t>
+  </si>
+  <si>
+    <t># of ID'd proteins</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -357,6 +378,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -399,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -413,6 +442,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +618,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'all data'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -613,7 +645,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$7</c:f>
+              <c:f>'all data'!$H$2:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -719,7 +751,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'all data'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -746,7 +778,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$7</c:f>
+              <c:f>'all data'!$I$2:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1118,7 +1150,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'all data'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1145,7 +1177,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:f>'all data'!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1574,7 +1606,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'all data'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1601,7 +1633,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$14:$H$19</c:f>
+              <c:f>'all data'!$H$14:$H$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1707,7 +1739,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'all data'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1734,7 +1766,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$14:$I$19</c:f>
+              <c:f>'all data'!$I$14:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2106,7 +2138,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'all data'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2133,7 +2165,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$14:$F$19</c:f>
+              <c:f>'all data'!$F$14:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2570,7 +2602,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$I$28:$I$30</c:f>
+              <c:f>'all data'!$I$28:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2588,7 +2620,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$28:$J$30</c:f>
+              <c:f>'all data'!$J$28:$J$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2685,7 +2717,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$I$28:$I$30</c:f>
+              <c:f>'all data'!$I$28:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2703,7 +2735,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$28:$K$30</c:f>
+              <c:f>'all data'!$K$28:$K$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3071,7 +3103,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$7</c:f>
+              <c:f>'all data'!$O$2:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3254,6 +3286,694 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" i="1"/>
+              <a:t>de novo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> only peptides</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>suspended (0.3-2.7 um)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="24000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="55000">
+                  <a:srgbClr val="0070C0"/>
+                </a:gs>
+              </a:gsLst>
+              <a:path path="circle">
+                <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+              </a:path>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>3377</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-8CD7-0E46-855D-35AF5E24CBE5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1655</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-8CD7-0E46-855D-35AF5E24CBE5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'100-965 comparison'!$D$3:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'100-965 comparison'!$B$3:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'100-965 comparison'!$C$3:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1655</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8CD7-0E46-855D-35AF5E24CBE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sinking</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="24000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="55000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:path path="circle">
+                <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+              </a:path>
+            </a:gradFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1175</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-8CD7-0E46-855D-35AF5E24CBE5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>6635</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-8CD7-0E46-855D-35AF5E24CBE5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'100-965 comparison'!$D$8:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'100-965 comparison'!$B$8:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'100-965 comparison'!$C$8:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6635</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8CD7-0E46-855D-35AF5E24CBE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="679452944"/>
+        <c:axId val="674288448"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="679452944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674288448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="679452944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -3497,6 +4217,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -6508,6 +7268,541 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6756,6 +8051,210 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33DA6BC9-8987-1548-9399-3D7087F0EEE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.2584</cdr:x>
+      <cdr:y>0.125</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.42526</cdr:x>
+      <cdr:y>0.19767</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD5E656-48EB-5247-A3D6-D31E1B0020CA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1416050" y="546100"/>
+          <a:ext cx="914400" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>suspended </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.69293</cdr:x>
+      <cdr:y>0.11919</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.85979</cdr:x>
+      <cdr:y>0.19186</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DCA4D0-3347-C647-BC53-7E8414DB7BEE}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3797300" y="520700"/>
+          <a:ext cx="914400" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>sinking </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7055,9 +8554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FAA684-DE3F-5A4C-BBF8-96E0D7E03E10}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7096,34 +8595,31 @@
         <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -7506,6 +9002,15 @@
       <c r="G8">
         <v>17310</v>
       </c>
+      <c r="H8">
+        <v>241</v>
+      </c>
+      <c r="I8">
+        <v>272</v>
+      </c>
+      <c r="J8">
+        <v>2313</v>
+      </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9">
@@ -7526,6 +9031,15 @@
       <c r="G9">
         <v>34506</v>
       </c>
+      <c r="H9">
+        <v>1538</v>
+      </c>
+      <c r="I9">
+        <v>1216</v>
+      </c>
+      <c r="J9">
+        <v>7561</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10">
@@ -7546,6 +9060,15 @@
       <c r="G10">
         <v>33351</v>
       </c>
+      <c r="H10">
+        <v>827</v>
+      </c>
+      <c r="I10">
+        <v>703</v>
+      </c>
+      <c r="J10">
+        <v>5766</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11">
@@ -7566,6 +9089,15 @@
       <c r="G11">
         <v>28443</v>
       </c>
+      <c r="H11">
+        <v>390</v>
+      </c>
+      <c r="I11">
+        <v>432</v>
+      </c>
+      <c r="J11">
+        <v>3867</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12">
@@ -7586,6 +9118,15 @@
       <c r="G12">
         <v>29256</v>
       </c>
+      <c r="H12">
+        <v>390</v>
+      </c>
+      <c r="I12">
+        <v>340</v>
+      </c>
+      <c r="J12">
+        <v>4263</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13">
@@ -7606,6 +9147,15 @@
       <c r="G13">
         <v>15893</v>
       </c>
+      <c r="H13">
+        <v>118</v>
+      </c>
+      <c r="I13">
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>1655</v>
+      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14">
@@ -7786,7 +9336,7 @@
         <v>264</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>94</v>
@@ -7815,7 +9365,7 @@
         <v>265</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>94</v>
@@ -7844,7 +9394,7 @@
         <v>266</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22">
         <v>265</v>
@@ -7873,7 +9423,7 @@
         <v>267</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>265</v>
@@ -7902,7 +9452,7 @@
         <v>268</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>965</v>
@@ -7931,7 +9481,7 @@
         <v>269</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25">
         <v>965</v>
@@ -7960,7 +9510,7 @@
         <v>270</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -7974,7 +9524,7 @@
         <v>271</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -8093,13 +9643,121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD91425-9F4A-7E4E-B842-3368493BFFE4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="50" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>3377</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>965</v>
+      </c>
+      <c r="C4">
+        <v>1655</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="50" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8">
+        <v>94</v>
+      </c>
+      <c r="C8">
+        <v>1175</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9">
+        <v>965</v>
+      </c>
+      <c r="C9">
+        <v>6635</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8120,233 +9778,233 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="32">
       <c r="A1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4">
         <v>57.021464999999999</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4">
         <v>0.984016</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4">
         <v>-1.032</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4">
         <v>-18.010565</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4">
         <v>14.015650000000001</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="4">
         <v>15.994915000000001</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4">
         <v>15.994915000000001</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4">
         <v>79.966329999999999</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="4">
         <v>79.966329999999999</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="4">
         <v>79.956819999999993</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="4">
         <v>383.22809999999998</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4">
         <v>27.994914999999999</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="4">
         <v>42.01</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="4">
         <v>37.96</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4">
         <v>21.98</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="4">
         <v>28.03</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="4">
         <v>14.02</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="4">
         <v>-15.99</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="4">
         <v>-17.03</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" s="4">
         <v>28.03</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made histrogram of med4 tag lengths
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-mclane-profile.xlsx
+++ b/analyses/etnp2017-p2-mclane-profile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9242B1C7-C365-2B42-ACBF-8BD655105410}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB18AF6F-5385-3C4A-B09E-1CA88EE7E029}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="5740" windowWidth="25600" windowHeight="14620" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ptm" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -451,13 +452,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1229,6 +1230,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-8818-604D-8D58-15736B6AF4BA}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1435,6 +1439,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-8818-604D-8D58-15736B6AF4BA}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4227,6 +4234,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-58A4-BA48-8A4F-7333A3B7BC9C}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4452,6 +4462,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-58A4-BA48-8A4F-7333A3B7BC9C}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4988,6 +5001,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-8F53-BD42-97DA-DF4E77D74157}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5207,6 +5223,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-8F53-BD42-97DA-DF4E77D74157}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5762,6 +5781,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-C137-C445-8F1B-A78A3B9A0F82}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5981,6 +6003,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-C137-C445-8F1B-A78A3B9A0F82}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -11940,16 +11965,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>679450</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13235,9 +13260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FAA684-DE3F-5A4C-BBF8-96E0D7E03E10}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13348,7 +13373,7 @@
         <v>0.1555122900949136</v>
       </c>
       <c r="O2">
-        <f>N2*100</f>
+        <f t="shared" ref="O2:O7" si="0">N2*100</f>
         <v>15.55122900949136</v>
       </c>
       <c r="R2" s="4">
@@ -13409,7 +13434,7 @@
         <v>0.15597722960151802</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O7" si="0">N3*100</f>
+        <f t="shared" si="0"/>
         <v>15.597722960151803</v>
       </c>
       <c r="R3" s="4">
@@ -14337,11 +14362,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -14393,19 +14418,19 @@
       <c r="B4">
         <v>265</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>2826</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>1170</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>1804</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>18899</v>
       </c>
     </row>
@@ -14433,11 +14458,11 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -14497,7 +14522,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B11">

</xml_diff>